<commit_message>
Graphs added BFS n DFS
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -404,7 +404,7 @@
         <v xml:space="preserve">Done [yes or no] </v>
       </c>
       <c r="F4" t="str">
-        <v>code</v>
+        <v>comments</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         <v>Find the Union and Intersection of the two sorted arrays.</v>
       </c>
       <c r="D11" t="str">
-        <v>&lt;-&gt;</v>
+        <v>yes</v>
       </c>
     </row>
     <row r="12">
@@ -502,7 +502,10 @@
         <v>Write a program to cyclically rotate an array by one.</v>
       </c>
       <c r="D12" t="str">
-        <v>&lt;-&gt;</v>
+        <v>yes</v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve">O(n) requires A Juggling Algorithm </v>
       </c>
     </row>
     <row r="13">

</xml_diff>